<commit_message>
updated Bulk CI attachments
</commit_message>
<xml_diff>
--- a/src/test/resources/Test Attachments/50 CI's (WithDuplicates)/50CIsXLSX.xlsx
+++ b/src/test/resources/Test Attachments/50 CI's (WithDuplicates)/50CIsXLSX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h_smi\OneDrive\Documents\TemplatesForBulkCITests\50 CI's (WithDuplicates)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\oneworkflow.automation\src\test\resources\Test Attachments\50 CI's (WithDuplicates)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_AD3A4934EECE07DE3A30AC543493327F250C57B5" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{F1D868D9-6DB0-4F5E-BE23-A101C3D6B8DC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361AD2D9-65AF-4C1D-B6A9-C4676A8E2AD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-104" yWindow="-104" windowWidth="29699" windowHeight="16197" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CIList" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>CI Name</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>NO_AC_AC-AKH902-350-1-404</t>
+  </si>
+  <si>
+    <t>DK_AAA_AAA02DK</t>
+  </si>
+  <si>
+    <t>dk gdpr purpose</t>
   </si>
 </sst>
 </file>
@@ -456,265 +462,265 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>25</v>
       </c>

</xml_diff>